<commit_message>
first check of AVE composition (+ minor change in Check Protocol)
</commit_message>
<xml_diff>
--- a/Plancheck/plancheck_data/check_protocol/v19/STEC foie DCA.xlsx
+++ b/Plancheck/plancheck_data/check_protocol/v19/STEC foie DCA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400"/>
   </bookViews>
   <sheets>
     <sheet name="General data" sheetId="1" r:id="rId1"/>
@@ -40,493 +40,493 @@
     <t>AAA_15605New</t>
   </si>
   <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>Normalisation mode</t>
+  </si>
+  <si>
+    <t>Prescription percentage</t>
+  </si>
+  <si>
+    <t>100.00% couvre 50.00% du volume cible</t>
+  </si>
+  <si>
+    <t>100% au point de référence</t>
+  </si>
+  <si>
+    <t>Acuros_15605New</t>
+  </si>
+  <si>
+    <t>EMC_15605</t>
+  </si>
+  <si>
+    <t>Enable gating</t>
+  </si>
+  <si>
+    <t>Oui</t>
+  </si>
+  <si>
+    <t>Non</t>
+  </si>
+  <si>
+    <t>Grele</t>
+  </si>
+  <si>
+    <t>CouchInterior</t>
+  </si>
+  <si>
+    <t>CouchSurface</t>
+  </si>
+  <si>
+    <t>HU</t>
+  </si>
+  <si>
+    <t>zzInt_ORFIT</t>
+  </si>
+  <si>
+    <t>zzExt_ORFIT</t>
+  </si>
+  <si>
+    <t>Contrainte 1</t>
+  </si>
+  <si>
+    <t>Contrainte 2</t>
+  </si>
+  <si>
+    <t>Contrainte 3</t>
+  </si>
+  <si>
+    <t>Contrainte 4</t>
+  </si>
+  <si>
+    <t>Contrainte 5</t>
+  </si>
+  <si>
+    <t>Contrainte 6</t>
+  </si>
+  <si>
+    <t>Contrainte 7</t>
+  </si>
+  <si>
+    <t>Contrainte 8</t>
+  </si>
+  <si>
+    <t>Contrainte 9</t>
+  </si>
+  <si>
+    <t>Contrainte 10</t>
+  </si>
+  <si>
+    <t>,,,</t>
+  </si>
+  <si>
+    <t>6X</t>
+  </si>
+  <si>
+    <t>6X-FFF</t>
+  </si>
+  <si>
+    <t>10X</t>
+  </si>
+  <si>
+    <t>10X-FFF</t>
+  </si>
+  <si>
+    <t>6E</t>
+  </si>
+  <si>
+    <t>9E</t>
+  </si>
+  <si>
+    <t>12E</t>
+  </si>
+  <si>
+    <t>CQ</t>
+  </si>
+  <si>
+    <t>PDIP</t>
+  </si>
+  <si>
+    <t>Octa4D</t>
+  </si>
+  <si>
+    <t>RUBY</t>
+  </si>
+  <si>
+    <t>Energie des faisceaux</t>
+  </si>
+  <si>
+    <t>Table de tolérance</t>
+  </si>
+  <si>
+    <t>thorax</t>
+  </si>
+  <si>
+    <t>pelvis</t>
+  </si>
+  <si>
+    <t>non fixe</t>
+  </si>
+  <si>
+    <t>RISQUE COLLISION</t>
+  </si>
+  <si>
+    <t>IMRT/STEREO</t>
+  </si>
+  <si>
+    <t>STEC OS</t>
+  </si>
+  <si>
+    <t>membre</t>
+  </si>
+  <si>
+    <t>GDE TOLERANCE</t>
+  </si>
+  <si>
+    <t>physique</t>
+  </si>
+  <si>
+    <t>sein</t>
+  </si>
+  <si>
+    <t>vertebre</t>
+  </si>
+  <si>
+    <t>ORFIT BLEU</t>
+  </si>
+  <si>
+    <t>tete et cou</t>
+  </si>
+  <si>
+    <t>DV</t>
+  </si>
+  <si>
+    <t>STIC</t>
+  </si>
+  <si>
+    <t>physique_0tolera</t>
+  </si>
+  <si>
+    <t>NTO</t>
+  </si>
+  <si>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>PO options</t>
+  </si>
+  <si>
+    <t>AirCavityCorrection</t>
+  </si>
+  <si>
+    <t>ApertureShapeController</t>
+  </si>
+  <si>
+    <t>AutoFeathering</t>
+  </si>
+  <si>
+    <t>ConvergenceMode</t>
+  </si>
+  <si>
+    <t>DoseResolution</t>
+  </si>
+  <si>
+    <t>DoseResolutionSRSAndHyperArc</t>
+  </si>
+  <si>
+    <t>FieldGrouping</t>
+  </si>
+  <si>
+    <t>Inhomog. Correction</t>
+  </si>
+  <si>
+    <t>MRLevelAtRestart</t>
+  </si>
+  <si>
+    <t>SmoothX</t>
+  </si>
+  <si>
+    <t>SmoothY</t>
+  </si>
+  <si>
+    <t>UseGPU</t>
+  </si>
+  <si>
+    <t>Off</t>
+  </si>
+  <si>
+    <t>Moderate</t>
+  </si>
+  <si>
+    <t>On</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>MR3</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>Mandatory</t>
+  </si>
+  <si>
+    <t>Algo options</t>
+  </si>
+  <si>
+    <t>CalculationGridSizeInCM</t>
+  </si>
+  <si>
+    <t>CalculationGridSizeInCMForSRSAndHyperArc</t>
+  </si>
+  <si>
+    <t>FieldNormalizationType</t>
+  </si>
+  <si>
+    <t>HeterogeneityCorrection</t>
+  </si>
+  <si>
+    <t>VMAT</t>
+  </si>
+  <si>
+    <t>DCA</t>
+  </si>
+  <si>
+    <t>IMRT</t>
+  </si>
+  <si>
+    <t>RTC</t>
+  </si>
+  <si>
+    <t>Electrons</t>
+  </si>
+  <si>
+    <t>Tomo</t>
+  </si>
+  <si>
+    <t>Hyperarc</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Priorité</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Stop</t>
+  </si>
+  <si>
+    <t>Abaissement</t>
+  </si>
+  <si>
+    <t>STEC foie DCA</t>
+  </si>
+  <si>
+    <t>Reins</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>ReinGche</t>
+  </si>
+  <si>
+    <t>ReinDt</t>
+  </si>
+  <si>
+    <t>PTV</t>
+  </si>
+  <si>
+    <t>Poumons</t>
+  </si>
+  <si>
+    <t>PoumonGche</t>
+  </si>
+  <si>
+    <t>PoumonDt</t>
+  </si>
+  <si>
+    <t>ParoiThoracique</t>
+  </si>
+  <si>
+    <t>Oesophage</t>
+  </si>
+  <si>
+    <t>GTV</t>
+  </si>
+  <si>
+    <t>grain1</t>
+  </si>
+  <si>
+    <t>grain2</t>
+  </si>
+  <si>
+    <t>grain3</t>
+  </si>
+  <si>
+    <t>Foie</t>
+  </si>
+  <si>
+    <t>Estomac</t>
+  </si>
+  <si>
+    <t>Duodenum</t>
+  </si>
+  <si>
+    <t>Colon</t>
+  </si>
+  <si>
+    <t>Coeur</t>
+  </si>
+  <si>
+    <t>Canal med</t>
+  </si>
+  <si>
+    <t>Aorte/v.cave</t>
+  </si>
+  <si>
+    <t>Canal biliaire</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Trachee</t>
+  </si>
+  <si>
+    <t>VesiculeBiliaire</t>
+  </si>
+  <si>
+    <t>ITV</t>
+  </si>
+  <si>
+    <t>CTV</t>
+  </si>
+  <si>
+    <t>Foie-GTV</t>
+  </si>
+  <si>
+    <t>Canal+5</t>
+  </si>
+  <si>
+    <t>PTV grain1</t>
+  </si>
+  <si>
+    <t>PTV grain2</t>
+  </si>
+  <si>
+    <t>PTV grain3</t>
+  </si>
+  <si>
+    <t>D2cm</t>
+  </si>
+  <si>
+    <t>D98%&gt;100%</t>
+  </si>
+  <si>
+    <t>D0,1cc&gt;110%</t>
+  </si>
+  <si>
+    <t>D0,1cc&lt;140%</t>
+  </si>
+  <si>
+    <t>D0,1cc&lt;80%</t>
+  </si>
+  <si>
+    <t>D0,5cc&lt;45Gy</t>
+  </si>
+  <si>
+    <t>V12,3Gy&lt;1,2cc</t>
+  </si>
+  <si>
+    <t>V18Gy&lt;0,25cc</t>
+  </si>
+  <si>
+    <t>D0,1cc&lt;22Gy</t>
+  </si>
+  <si>
+    <t>Cœur</t>
+  </si>
+  <si>
+    <t>D0,5cc&lt;24Gy</t>
+  </si>
+  <si>
+    <t>D0,5cc&lt;28,2Gy</t>
+  </si>
+  <si>
+    <t>D0,5cc&lt;50Gy</t>
+  </si>
+  <si>
+    <t>V16,5Gy&lt;5cc</t>
+  </si>
+  <si>
+    <t>V11,4Gy&lt;10cc</t>
+  </si>
+  <si>
+    <t>D0,5cc&lt;22,2Gy</t>
+  </si>
+  <si>
+    <t>V16,5Gy&lt;10cc</t>
+  </si>
+  <si>
+    <t>D0,1cc&lt;22,2Gy</t>
+  </si>
+  <si>
+    <t>V15Gy&lt;50%</t>
+  </si>
+  <si>
+    <t>V17,7Gy&lt;5cc</t>
+  </si>
+  <si>
+    <t>D0,5cc&lt;25,2Gy</t>
+  </si>
+  <si>
+    <t>V21Gy&lt;5cc</t>
+  </si>
+  <si>
+    <t>Paroi Thoracique</t>
+  </si>
+  <si>
+    <t>V30Gy&lt;30cc</t>
+  </si>
+  <si>
+    <t>D0,5cc&lt;37Gy</t>
+  </si>
+  <si>
+    <t>Planning</t>
+  </si>
+  <si>
+    <t>PTV_HAUTE_DOSE</t>
+  </si>
+  <si>
+    <t>PTV_AUTRES</t>
+  </si>
+  <si>
     <t>100% to isocenter</t>
-  </si>
-  <si>
-    <t>ON</t>
-  </si>
-  <si>
-    <t>Normalisation mode</t>
-  </si>
-  <si>
-    <t>Prescription percentage</t>
-  </si>
-  <si>
-    <t>100.00% couvre 50.00% du volume cible</t>
-  </si>
-  <si>
-    <t>100% au point de référence</t>
-  </si>
-  <si>
-    <t>Acuros_15605New</t>
-  </si>
-  <si>
-    <t>EMC_15605</t>
-  </si>
-  <si>
-    <t>Enable gating</t>
-  </si>
-  <si>
-    <t>Oui</t>
-  </si>
-  <si>
-    <t>Non</t>
-  </si>
-  <si>
-    <t>Grele</t>
-  </si>
-  <si>
-    <t>CouchInterior</t>
-  </si>
-  <si>
-    <t>CouchSurface</t>
-  </si>
-  <si>
-    <t>HU</t>
-  </si>
-  <si>
-    <t>zzInt_ORFIT</t>
-  </si>
-  <si>
-    <t>zzExt_ORFIT</t>
-  </si>
-  <si>
-    <t>Contrainte 1</t>
-  </si>
-  <si>
-    <t>Contrainte 2</t>
-  </si>
-  <si>
-    <t>Contrainte 3</t>
-  </si>
-  <si>
-    <t>Contrainte 4</t>
-  </si>
-  <si>
-    <t>Contrainte 5</t>
-  </si>
-  <si>
-    <t>Contrainte 6</t>
-  </si>
-  <si>
-    <t>Contrainte 7</t>
-  </si>
-  <si>
-    <t>Contrainte 8</t>
-  </si>
-  <si>
-    <t>Contrainte 9</t>
-  </si>
-  <si>
-    <t>Contrainte 10</t>
-  </si>
-  <si>
-    <t>,,,</t>
-  </si>
-  <si>
-    <t>6X</t>
-  </si>
-  <si>
-    <t>6X-FFF</t>
-  </si>
-  <si>
-    <t>10X</t>
-  </si>
-  <si>
-    <t>10X-FFF</t>
-  </si>
-  <si>
-    <t>6E</t>
-  </si>
-  <si>
-    <t>9E</t>
-  </si>
-  <si>
-    <t>12E</t>
-  </si>
-  <si>
-    <t>CQ</t>
-  </si>
-  <si>
-    <t>PDIP</t>
-  </si>
-  <si>
-    <t>Octa4D</t>
-  </si>
-  <si>
-    <t>RUBY</t>
-  </si>
-  <si>
-    <t>Energie des faisceaux</t>
-  </si>
-  <si>
-    <t>Table de tolérance</t>
-  </si>
-  <si>
-    <t>thorax</t>
-  </si>
-  <si>
-    <t>pelvis</t>
-  </si>
-  <si>
-    <t>non fixe</t>
-  </si>
-  <si>
-    <t>RISQUE COLLISION</t>
-  </si>
-  <si>
-    <t>IMRT/STEREO</t>
-  </si>
-  <si>
-    <t>STEC OS</t>
-  </si>
-  <si>
-    <t>membre</t>
-  </si>
-  <si>
-    <t>GDE TOLERANCE</t>
-  </si>
-  <si>
-    <t>physique</t>
-  </si>
-  <si>
-    <t>sein</t>
-  </si>
-  <si>
-    <t>vertebre</t>
-  </si>
-  <si>
-    <t>ORFIT BLEU</t>
-  </si>
-  <si>
-    <t>tete et cou</t>
-  </si>
-  <si>
-    <t>DV</t>
-  </si>
-  <si>
-    <t>STIC</t>
-  </si>
-  <si>
-    <t>physique_0tolera</t>
-  </si>
-  <si>
-    <t>NTO</t>
-  </si>
-  <si>
-    <t>Auto</t>
-  </si>
-  <si>
-    <t>Manual</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>PO options</t>
-  </si>
-  <si>
-    <t>AirCavityCorrection</t>
-  </si>
-  <si>
-    <t>ApertureShapeController</t>
-  </si>
-  <si>
-    <t>AutoFeathering</t>
-  </si>
-  <si>
-    <t>ConvergenceMode</t>
-  </si>
-  <si>
-    <t>DoseResolution</t>
-  </si>
-  <si>
-    <t>DoseResolutionSRSAndHyperArc</t>
-  </si>
-  <si>
-    <t>FieldGrouping</t>
-  </si>
-  <si>
-    <t>Inhomog. Correction</t>
-  </si>
-  <si>
-    <t>MRLevelAtRestart</t>
-  </si>
-  <si>
-    <t>SmoothX</t>
-  </si>
-  <si>
-    <t>SmoothY</t>
-  </si>
-  <si>
-    <t>UseGPU</t>
-  </si>
-  <si>
-    <t>Off</t>
-  </si>
-  <si>
-    <t>Moderate</t>
-  </si>
-  <si>
-    <t>On</t>
-  </si>
-  <si>
-    <t>Normal</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>MR3</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>3.0</t>
-  </si>
-  <si>
-    <t>Mandatory</t>
-  </si>
-  <si>
-    <t>Algo options</t>
-  </si>
-  <si>
-    <t>CalculationGridSizeInCM</t>
-  </si>
-  <si>
-    <t>CalculationGridSizeInCMForSRSAndHyperArc</t>
-  </si>
-  <si>
-    <t>FieldNormalizationType</t>
-  </si>
-  <si>
-    <t>HeterogeneityCorrection</t>
-  </si>
-  <si>
-    <t>VMAT</t>
-  </si>
-  <si>
-    <t>DCA</t>
-  </si>
-  <si>
-    <t>IMRT</t>
-  </si>
-  <si>
-    <t>RTC</t>
-  </si>
-  <si>
-    <t>Electrons</t>
-  </si>
-  <si>
-    <t>Tomo</t>
-  </si>
-  <si>
-    <t>Hyperarc</t>
-  </si>
-  <si>
-    <t>Mode</t>
-  </si>
-  <si>
-    <t>Priorité</t>
-  </si>
-  <si>
-    <t>Distance</t>
-  </si>
-  <si>
-    <t>Start</t>
-  </si>
-  <si>
-    <t>Stop</t>
-  </si>
-  <si>
-    <t>Abaissement</t>
-  </si>
-  <si>
-    <t>STEC foie DCA</t>
-  </si>
-  <si>
-    <t>Reins</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>ReinGche</t>
-  </si>
-  <si>
-    <t>ReinDt</t>
-  </si>
-  <si>
-    <t>PTV</t>
-  </si>
-  <si>
-    <t>Poumons</t>
-  </si>
-  <si>
-    <t>PoumonGche</t>
-  </si>
-  <si>
-    <t>PoumonDt</t>
-  </si>
-  <si>
-    <t>ParoiThoracique</t>
-  </si>
-  <si>
-    <t>Oesophage</t>
-  </si>
-  <si>
-    <t>GTV</t>
-  </si>
-  <si>
-    <t>grain1</t>
-  </si>
-  <si>
-    <t>grain2</t>
-  </si>
-  <si>
-    <t>grain3</t>
-  </si>
-  <si>
-    <t>Foie</t>
-  </si>
-  <si>
-    <t>Estomac</t>
-  </si>
-  <si>
-    <t>Duodenum</t>
-  </si>
-  <si>
-    <t>Colon</t>
-  </si>
-  <si>
-    <t>Coeur</t>
-  </si>
-  <si>
-    <t>Canal med</t>
-  </si>
-  <si>
-    <t>Aorte/v.cave</t>
-  </si>
-  <si>
-    <t>Canal biliaire</t>
-  </si>
-  <si>
-    <t>Rate</t>
-  </si>
-  <si>
-    <t>Trachee</t>
-  </si>
-  <si>
-    <t>VesiculeBiliaire</t>
-  </si>
-  <si>
-    <t>ITV</t>
-  </si>
-  <si>
-    <t>CTV</t>
-  </si>
-  <si>
-    <t>Foie-GTV</t>
-  </si>
-  <si>
-    <t>Canal+5</t>
-  </si>
-  <si>
-    <t>PTV grain1</t>
-  </si>
-  <si>
-    <t>PTV grain2</t>
-  </si>
-  <si>
-    <t>PTV grain3</t>
-  </si>
-  <si>
-    <t>D2cm</t>
-  </si>
-  <si>
-    <t>D98%&gt;100%</t>
-  </si>
-  <si>
-    <t>D0,1cc&gt;110%</t>
-  </si>
-  <si>
-    <t>D0,1cc&lt;140%</t>
-  </si>
-  <si>
-    <t>D0,1cc&lt;80%</t>
-  </si>
-  <si>
-    <t>D0,5cc&lt;45Gy</t>
-  </si>
-  <si>
-    <t>V12,3Gy&lt;1,2cc</t>
-  </si>
-  <si>
-    <t>V18Gy&lt;0,25cc</t>
-  </si>
-  <si>
-    <t>D0,1cc&lt;22Gy</t>
-  </si>
-  <si>
-    <t>Cœur</t>
-  </si>
-  <si>
-    <t>D0,5cc&lt;24Gy</t>
-  </si>
-  <si>
-    <t>D0,5cc&lt;28,2Gy</t>
-  </si>
-  <si>
-    <t>D0,5cc&lt;50Gy</t>
-  </si>
-  <si>
-    <t>V16,5Gy&lt;5cc</t>
-  </si>
-  <si>
-    <t>V11,4Gy&lt;10cc</t>
-  </si>
-  <si>
-    <t>D0,5cc&lt;22,2Gy</t>
-  </si>
-  <si>
-    <t>V16,5Gy&lt;10cc</t>
-  </si>
-  <si>
-    <t>D0,1cc&lt;22,2Gy</t>
-  </si>
-  <si>
-    <t>V15Gy&lt;50%</t>
-  </si>
-  <si>
-    <t>V17,7Gy&lt;5cc</t>
-  </si>
-  <si>
-    <t>D0,5cc&lt;25,2Gy</t>
-  </si>
-  <si>
-    <t>V21Gy&lt;5cc</t>
-  </si>
-  <si>
-    <t>Paroi Thoracique</t>
-  </si>
-  <si>
-    <t>V30Gy&lt;30cc</t>
-  </si>
-  <si>
-    <t>D0,5cc&lt;37Gy</t>
-  </si>
-  <si>
-    <t>Planning</t>
-  </si>
-  <si>
-    <t>PTV_HAUTE_DOSE</t>
-  </si>
-  <si>
-    <t>PTV_AUTRES</t>
   </si>
 </sst>
 </file>
@@ -1516,8 +1516,8 @@
   </sheetPr>
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1539,7 +1539,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C1" s="18"/>
       <c r="D1" s="18"/>
@@ -1574,7 +1574,7 @@
       <c r="G3" s="18"/>
       <c r="H3" s="19"/>
       <c r="L3" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1591,12 +1591,12 @@
       <c r="G4" s="18"/>
       <c r="H4" s="19"/>
       <c r="L4" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="21">
         <v>0.8</v>
@@ -1610,10 +1610,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
@@ -1622,15 +1622,15 @@
       <c r="G6" s="18"/>
       <c r="H6" s="19"/>
       <c r="L6" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>13</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>14</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
@@ -1639,15 +1639,15 @@
       <c r="G7" s="18"/>
       <c r="H7" s="19"/>
       <c r="L7" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
@@ -1658,10 +1658,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>40</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>41</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
@@ -1670,15 +1670,15 @@
       <c r="G9" s="18"/>
       <c r="H9" s="19"/>
       <c r="L9" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="18" t="s">
         <v>45</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>46</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
@@ -1687,7 +1687,7 @@
       <c r="G10" s="18"/>
       <c r="H10" s="19"/>
       <c r="L10" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1717,7 +1717,7 @@
       <c r="G13" s="32"/>
       <c r="H13" s="33"/>
       <c r="L13" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1729,7 +1729,7 @@
       <c r="G14" s="32"/>
       <c r="H14" s="33"/>
       <c r="L14" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1741,12 +1741,12 @@
       <c r="G15" s="32"/>
       <c r="H15" s="33"/>
       <c r="L15" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="33"/>
@@ -1756,15 +1756,15 @@
       <c r="G16" s="32"/>
       <c r="H16" s="33"/>
       <c r="L16" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C17" s="31"/>
       <c r="D17" s="30"/>
@@ -1773,15 +1773,15 @@
       <c r="G17" s="30"/>
       <c r="H17" s="31"/>
       <c r="L17" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C18" s="31"/>
       <c r="D18" s="30"/>
@@ -1790,15 +1790,15 @@
       <c r="G18" s="30"/>
       <c r="H18" s="31"/>
       <c r="L18" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C19" s="31"/>
       <c r="D19" s="30"/>
@@ -1807,15 +1807,15 @@
       <c r="G19" s="30"/>
       <c r="H19" s="31"/>
       <c r="L19" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C20" s="31"/>
       <c r="D20" s="30"/>
@@ -1826,10 +1826,10 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C21" s="31"/>
       <c r="D21" s="30"/>
@@ -1838,15 +1838,15 @@
       <c r="G21" s="30"/>
       <c r="H21" s="31"/>
       <c r="L21" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C22" s="31"/>
       <c r="D22" s="30"/>
@@ -1855,15 +1855,15 @@
       <c r="G22" s="30"/>
       <c r="H22" s="31"/>
       <c r="L22" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C23" s="31"/>
       <c r="D23" s="30"/>
@@ -1872,15 +1872,15 @@
       <c r="G23" s="30"/>
       <c r="H23" s="31"/>
       <c r="L23" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C24" s="31"/>
       <c r="D24" s="30"/>
@@ -1891,10 +1891,10 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C25" s="31"/>
       <c r="D25" s="30"/>
@@ -1905,7 +1905,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B26" s="30">
         <v>200</v>
@@ -1917,12 +1917,12 @@
       <c r="G26" s="30"/>
       <c r="H26" s="31"/>
       <c r="L26" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B27" s="30">
         <v>200</v>
@@ -1934,15 +1934,15 @@
       <c r="G27" s="30"/>
       <c r="H27" s="31"/>
       <c r="L27" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C28" s="30"/>
       <c r="D28" s="30"/>
@@ -1951,7 +1951,7 @@
       <c r="G28" s="30"/>
       <c r="H28" s="30"/>
       <c r="L28" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -1963,12 +1963,12 @@
       <c r="G29" s="32"/>
       <c r="H29" s="32"/>
       <c r="L29" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B30" s="32"/>
       <c r="C30" s="32"/>
@@ -1978,7 +1978,7 @@
       <c r="G30" s="32"/>
       <c r="H30" s="32"/>
       <c r="L30" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -1995,12 +1995,12 @@
       <c r="G31" s="27"/>
       <c r="H31" s="27"/>
       <c r="L31" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B32" s="27">
         <v>0.125</v>
@@ -2012,12 +2012,12 @@
       <c r="G32" s="27"/>
       <c r="H32" s="27"/>
       <c r="L32" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B33" s="27">
         <v>0.125</v>
@@ -2029,15 +2029,15 @@
       <c r="G33" s="27"/>
       <c r="H33" s="27"/>
       <c r="L33" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>5</v>
+        <v>167</v>
       </c>
       <c r="C34" s="27"/>
       <c r="D34" s="27"/>
@@ -2046,15 +2046,15 @@
       <c r="G34" s="27"/>
       <c r="H34" s="27"/>
       <c r="L34" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C35" s="27"/>
       <c r="D35" s="27"/>
@@ -2063,7 +2063,7 @@
       <c r="G35" s="27"/>
       <c r="H35" s="27"/>
       <c r="L35" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -2076,7 +2076,7 @@
       <c r="G36" s="27"/>
       <c r="H36" s="27"/>
       <c r="L36" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2089,7 +2089,7 @@
       <c r="G37" s="27"/>
       <c r="H37" s="27"/>
       <c r="L37" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -2102,7 +2102,7 @@
       <c r="G38" s="27"/>
       <c r="H38" s="27"/>
       <c r="L38" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -2115,7 +2115,7 @@
       <c r="G39" s="27"/>
       <c r="H39" s="27"/>
       <c r="L39" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -2128,7 +2128,7 @@
       <c r="G40" s="27"/>
       <c r="H40" s="27"/>
       <c r="L40" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -2141,20 +2141,20 @@
       <c r="G41" s="27"/>
       <c r="H41" s="27"/>
       <c r="L41" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C44" s="24"/>
       <c r="D44" s="24"/>
@@ -2165,7 +2165,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B45" s="23">
         <v>300</v>
@@ -2179,7 +2179,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B46" s="23">
         <v>3</v>
@@ -2193,7 +2193,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B47" s="23">
         <v>100</v>
@@ -2207,7 +2207,7 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B48" s="23">
         <v>30</v>
@@ -2219,12 +2219,12 @@
       <c r="G48" s="24"/>
       <c r="H48" s="24"/>
       <c r="L48" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B49" s="23">
         <v>0.1</v>
@@ -2236,52 +2236,52 @@
       <c r="G49" s="24"/>
       <c r="H49" s="24"/>
       <c r="L49" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L51" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L52" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L55" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L56" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L57" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L58" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L59" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L60" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L61" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2338,208 +2338,208 @@
         <v>2</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>108</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2569,67 +2569,67 @@
         <v>2</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2658,54 +2658,54 @@
         <v>2</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="6">
         <v>-1000</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="6">
         <v>-300</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="6">
         <v>0</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="6">
         <v>-900</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2720,7 +2720,7 @@
   </sheetPr>
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -2737,192 +2737,192 @@
         <v>2</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="D1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="E1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>31</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C2" s="34"/>
       <c r="D2" s="34"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B4" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="D4" s="34" t="s">
         <v>147</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" s="34" t="s">
         <v>149</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>150</v>
       </c>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B8" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="D8" s="34" t="s">
         <v>154</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B9" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="C9" s="34" t="s">
         <v>156</v>
-      </c>
-      <c r="C9" s="34" t="s">
-        <v>157</v>
       </c>
       <c r="D9" s="34"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C10" s="34"/>
       <c r="D10" s="34"/>
     </row>
     <row r="11" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="C11" s="34" t="s">
         <v>159</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>160</v>
       </c>
       <c r="D11" s="34"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D12" s="34"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B13" s="34" t="s">
         <v>162</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="C13" s="34" t="s">
         <v>163</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>164</v>
       </c>
       <c r="D13" s="34"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B15" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="C15" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="D15" s="34" t="s">
         <v>142</v>
-      </c>
-      <c r="D15" s="34" t="s">
-        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>